<commit_message>
Agregando licitacion de requisitos
</commit_message>
<xml_diff>
--- a/NV/Desarrollo/SBDL/Requisitos/SBDL_ER.xlsx
+++ b/NV/Desarrollo/SBDL/Requisitos/SBDL_ER.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Desktop\UNMSM\IX CICLO\GESTION DE LA CONFIG\unmsm_G4\NV\Desarrollo\SBDL\Requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="ITERACION1" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ITERACION1!$B$3:$F$3</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>LISTA DE REQUISITOS DEL SISTEMA XYZ</t>
   </si>
@@ -50,24 +51,9 @@
     <t>RQ01</t>
   </si>
   <si>
-    <t>VENTAS</t>
-  </si>
-  <si>
-    <t>Vendedor</t>
-  </si>
-  <si>
-    <t>Registrar Cliente</t>
-  </si>
-  <si>
-    <t>El sistema debe permitir registra los datos del cliente, tales como: Apellidos paterno, materno, tipo de documento de identidad, numero de documento de identidad, ….</t>
-  </si>
-  <si>
     <t>RQ02</t>
   </si>
   <si>
-    <t>CU01- Mantenimiento de clientes</t>
-  </si>
-  <si>
     <t>RQ03</t>
   </si>
   <si>
@@ -122,50 +108,107 @@
     <t>RQ20</t>
   </si>
   <si>
-    <t>Modificar datos del cliente</t>
-  </si>
-  <si>
-    <t>Actualizar datos de clientes</t>
-  </si>
-  <si>
     <t>Nombre de Caso de Uso</t>
   </si>
   <si>
     <t>Nombre Requisito</t>
   </si>
   <si>
-    <t>Modificar Datos de Clientes</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prototipo </t>
   </si>
   <si>
-    <t xml:space="preserve">Prototipo 001: Mantenimiento de Clientes </t>
-  </si>
-  <si>
-    <t>PROTOTIPO-001</t>
-  </si>
-  <si>
-    <t>COMPRAS</t>
-  </si>
-  <si>
-    <t>AISTENTE COMPRAS</t>
-  </si>
-  <si>
-    <t>Registrar COMPRAS</t>
-  </si>
-  <si>
     <t>ELISITACIÓN DE REQUISITOS</t>
+  </si>
+  <si>
+    <t>LISTA DE REQUISITOS DEL SISTEMA SBDL</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Evaluar curso del docente</t>
+  </si>
+  <si>
+    <t>Comentar curso del docente</t>
+  </si>
+  <si>
+    <t>Ver Detalles del curso del docente</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario valorar el nivel del curso del docente, asignandole a este una calificaciòn de 1 a 5 estrellas</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario brindar al usuario comentarios acerca del curso del docente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe mostrar al usuario los detalles del docente, tales como:  Nombre del Docente, Informacion de la direccion, Informacion acadèmica. </t>
+  </si>
+  <si>
+    <t>Valoracion</t>
+  </si>
+  <si>
+    <t>Registro</t>
+  </si>
+  <si>
+    <t>Registrar Alumno</t>
+  </si>
+  <si>
+    <t>Registrar docente</t>
+  </si>
+  <si>
+    <t>Alumno</t>
+  </si>
+  <si>
+    <t>Docente</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir registrar a un usuario con una información básica: Nombre de usuario, Nombres y apellidos, Contraseña, Correo electrónico, puede registrarse como máximo un usuario por cada correo electronico, registrándolo con el perfil de tipo Alumno</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir registrar a un usuario con una información básica: Nombre de usuario, Nombres y apellidos, Contraseña, Correo electrónico, puede registrarse como máximo un usuario por cada correo electronico, registrándolo con el perfil de tipo Docente</t>
+  </si>
+  <si>
+    <t>Acceso</t>
+  </si>
+  <si>
+    <t>Docente, Alumno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login </t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario, sea docente o alumno, logearse al sistema, con un usuario y una contraseña que ingreso anteriormente el usuario para registrarse al sistema.</t>
+  </si>
+  <si>
+    <t>Buscar Docente</t>
+  </si>
+  <si>
+    <t>Docente,Alumno</t>
+  </si>
+  <si>
+    <t>Busqueda</t>
+  </si>
+  <si>
+    <t>El usuario debe poder buscar a los docentes registrados en el sistema, filtrando por nombres, apellidos, cursos que dicta el profesor, etc.</t>
+  </si>
+  <si>
+    <t>Agregar</t>
+  </si>
+  <si>
+    <t>Agregar curso al docente</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario docente agregar el curso que desee dictar a sus alumnos. El curso debe tener todos los detalles que pide el sistema, como categoria, nivel, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo 001: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -192,13 +235,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -212,9 +248,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -232,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -312,17 +347,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -417,13 +441,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -442,78 +496,70 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="justify"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
-    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -599,43 +645,6 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>97702</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>590551</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="1 Imagen"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="11296" t="31001" r="44396" b="13626"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="428625" y="859702"/>
-          <a:ext cx="5267326" cy="3702774"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -928,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -939,285 +948,506 @@
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
     <col min="6" max="6" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="16" t="s">
+      <c r="E5" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+    </row>
+    <row r="8" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="13" t="s">
+      <c r="F18" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+    </row>
+    <row r="20" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="15"/>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="15"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="15"/>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="15"/>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="15"/>
+      <c r="C21" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="21"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+    </row>
+    <row r="23" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="22"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+    </row>
+    <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="20"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="21"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="22"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="20"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+    </row>
+    <row r="28" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="21"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+    </row>
+    <row r="29" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="22"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+    </row>
+    <row r="30" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+    </row>
+    <row r="31" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+    </row>
+    <row r="35" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+    </row>
+    <row r="37" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+    </row>
+    <row r="38" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+    </row>
+    <row r="39" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+    </row>
+    <row r="40" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+    </row>
+    <row r="41" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+    </row>
+    <row r="42" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+    </row>
+    <row r="43" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+    </row>
+    <row r="44" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="B3:F3"/>
-  <mergeCells count="2">
+  <mergeCells count="67">
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="D15:D17"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1225,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1243,14 +1473,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1265,144 +1495,126 @@
     </row>
     <row r="3" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="18" t="s">
+      <c r="G3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="32">
-        <v>2</v>
-      </c>
-      <c r="I4" s="24" t="s">
-        <v>40</v>
-      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="25"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="26"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="19"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="19"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="19"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="19"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1410,12 +1622,12 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="19"/>
+      <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1423,12 +1635,12 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="19"/>
+      <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -1436,12 +1648,12 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="19"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1449,12 +1661,12 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="19"/>
+      <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1462,12 +1674,12 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="19"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1475,12 +1687,12 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="19"/>
+      <c r="I16" s="16"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1488,12 +1700,12 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="19"/>
+      <c r="I17" s="16"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1501,12 +1713,12 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="19"/>
+      <c r="I18" s="16"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1514,12 +1726,12 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="19"/>
+      <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1527,12 +1739,12 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="19"/>
+      <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1540,12 +1752,12 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="19"/>
+      <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1553,12 +1765,12 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="19"/>
+      <c r="I22" s="16"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1566,16 +1778,11 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="19"/>
+      <c r="I23" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="I4:I6"/>
+  <mergeCells count="1">
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1586,7 +1793,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1622,7 +1829,7 @@
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>

</xml_diff>

<commit_message>
Terminando licitacion de requisitos
</commit_message>
<xml_diff>
--- a/NV/Desarrollo/SBDL/Requisitos/SBDL_ER.xlsx
+++ b/NV/Desarrollo/SBDL/Requisitos/SBDL_ER.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ITERACION1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
   <si>
     <t>LISTA DE REQUISITOS DEL SISTEMA XYZ</t>
   </si>
@@ -199,6 +199,48 @@
   </si>
   <si>
     <t>El sistema debe permitir al usuario docente agregar el curso que desee dictar a sus alumnos. El curso debe tener todos los detalles que pide el sistema, como categoria, nivel, etc.</t>
+  </si>
+  <si>
+    <t>Actualizacion</t>
+  </si>
+  <si>
+    <t>Actualizar datos del docente</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario docente actualizar sus datos personales, tales como biografia, nombres y apellidos, etc.</t>
+  </si>
+  <si>
+    <t>Eliminar curso al docente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agrega curso favorito </t>
+  </si>
+  <si>
+    <t>Eliminar curso favorito</t>
+  </si>
+  <si>
+    <t>Agregar cursos buscados al historial</t>
+  </si>
+  <si>
+    <t>Eliminar historial de busqueda</t>
+  </si>
+  <si>
+    <t>Eliminar</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario alumno poder eliminar el historial de busqueda que se le muestra al inicio.</t>
+  </si>
+  <si>
+    <t>Se debe generar un historial de busqueda a traves del tiempo del usuario alumno</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario alumno eliminar un curso de la lista de favoritos que tenga.</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario docente agregar un curso a la lista de favoritos quer posee un alumno en su perfil.</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario docente eliminar el curso que desee dictar a sus alumnos.</t>
   </si>
   <si>
     <t xml:space="preserve">Prototipo 001: </t>
@@ -527,6 +569,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -543,18 +597,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -939,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -954,21 +996,21 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
     </row>
@@ -1031,34 +1073,34 @@
       <c r="B6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="30" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="21"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="22"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
@@ -1133,7 +1175,7 @@
       <c r="B15" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="24" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="20" t="s">
@@ -1149,7 +1191,7 @@
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="21"/>
-      <c r="C16" s="30"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
@@ -1157,7 +1199,7 @@
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="22"/>
-      <c r="C17" s="31"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
@@ -1201,81 +1243,111 @@
       <c r="B21" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="23" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="21"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="22"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
     </row>
     <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="20"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="21"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-    </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+    </row>
+    <row r="26" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="22"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="20"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-    </row>
-    <row r="28" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="21"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-    </row>
-    <row r="29" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+    </row>
+    <row r="29" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="22"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
     </row>
     <row r="30" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
+      <c r="B30" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="21"/>
@@ -1284,19 +1356,29 @@
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
+    <row r="33" spans="2:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="34" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="21"/>
@@ -1313,11 +1395,21 @@
       <c r="F35" s="22"/>
     </row>
     <row r="36" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
+      <c r="B36" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="37" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="21"/>
@@ -1326,7 +1418,7 @@
       <c r="E37" s="21"/>
       <c r="F37" s="21"/>
     </row>
-    <row r="38" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
@@ -1334,11 +1426,21 @@
       <c r="F38" s="22"/>
     </row>
     <row r="39" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
+      <c r="B39" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="40" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="21"/>
@@ -1347,7 +1449,7 @@
       <c r="E40" s="21"/>
       <c r="F40" s="21"/>
     </row>
-    <row r="41" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
@@ -1355,11 +1457,21 @@
       <c r="F41" s="22"/>
     </row>
     <row r="42" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
+      <c r="B42" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="43" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="21"/>
@@ -1368,7 +1480,7 @@
       <c r="E43" s="21"/>
       <c r="F43" s="21"/>
     </row>
-    <row r="44" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
@@ -1378,57 +1490,6 @@
   </sheetData>
   <autoFilter ref="B3:F3"/>
   <mergeCells count="67">
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F21:F23"/>
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="D15:D17"/>
@@ -1445,6 +1506,57 @@
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="F42:F44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1473,14 +1585,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1792,7 +1904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1829,7 +1941,7 @@
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>

</xml_diff>